<commit_message>
implemented Data Driven concept- for TestCases.TC003_CreateAccount_DataDrivenTest using Excel file for Test Data and Data provider to provide the data to test classes
</commit_message>
<xml_diff>
--- a/src/test/TestData/MyStoreTestData.xlsx
+++ b/src/test/TestData/MyStoreTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareTesting\Workspaces\RealTimeProject\Automation_Framework_E-Commerce\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A197678-BE71-406D-A7F5-6AD3DBF00E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646C8038-F534-4660-B9DE-57754B3E5A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="870" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Email</t>
   </si>
@@ -49,17 +49,44 @@
     <t>Anant_Test@mailinator.com</t>
   </si>
   <si>
-    <t>QA Automation</t>
-  </si>
-  <si>
     <t>test1234!</t>
+  </si>
+  <si>
+    <t>Anant Automation</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>Welcome, Anant Kumar!</t>
+  </si>
+  <si>
+    <t>Thank you for registering with Main Website Store.</t>
+  </si>
+  <si>
+    <t>Anant</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Thank You Message </t>
+  </si>
+  <si>
+    <t>QA2_Test@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +114,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -109,10 +151,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -396,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,14 +454,14 @@
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -435,10 +481,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -456,14 +502,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8876E9E4-C80E-4198-AF6F-17F82CC2F470}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{4BE6A750-20E1-4CF9-9888-9B9AA0F3D5C7}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{6AA5A876-368E-48FB-BEDA-6F618AC721AE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>